<commit_message>
horario actualizado 31 de agosto
</commit_message>
<xml_diff>
--- a/4_semestre/horario.xlsx
+++ b/4_semestre/horario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Lunes</t>
   </si>
@@ -115,10 +115,6 @@
   <si>
     <t>Clase 
 secc 2</t>
-  </si>
-  <si>
-    <t>Clase 
-secc 1</t>
   </si>
   <si>
     <t>Arquitectura de
@@ -556,7 +552,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,9 +662,7 @@
       <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
@@ -684,9 +678,7 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="D8" s="8"/>
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
@@ -697,14 +689,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -712,14 +704,14 @@
         <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
horario actualizado-clase 5 fisica- informe 1 arquitectura- infrome modulo
</commit_message>
<xml_diff>
--- a/4_semestre/horario.xlsx
+++ b/4_semestre/horario.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricardo\Documents\A-U\4_semestre\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3787F83-7A88-4410-B1AF-0545FB4D5F6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28515" windowHeight="12855"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>Lunes</t>
   </si>
@@ -113,10 +119,6 @@
 SALA 15</t>
   </si>
   <si>
-    <t>Clase 
-secc 2</t>
-  </si>
-  <si>
     <t>Arquitectura de
 computadores
 LAB</t>
@@ -125,12 +127,21 @@
     <t>Logica para ciencias
 de la computacion
 SALA 19</t>
+  </si>
+  <si>
+    <t>Programacion 
+Avanzada 
+LAB</t>
+  </si>
+  <si>
+    <t>Ayudantia 
+Calculo III</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,12 +204,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -243,9 +248,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -257,6 +259,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -305,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,9 +343,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,6 +395,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,11 +587,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,6 +659,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -627,9 +669,7 @@
       <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="F4" s="8"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -646,9 +686,7 @@
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -662,7 +700,9 @@
       <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
@@ -678,7 +718,9 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
@@ -689,14 +731,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,14 +746,14 @@
         <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -732,7 +774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -744,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se actualizo el horario 04-10-2019
</commit_message>
<xml_diff>
--- a/4_semestre/horario.xlsx
+++ b/4_semestre/horario.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricardo\Documents\A-U\4_semestre\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3787F83-7A88-4410-B1AF-0545FB4D5F6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Lunes</t>
   </si>
@@ -107,10 +101,6 @@
 SALA 32</t>
   </si>
   <si>
-    <t>Algebra ii
-aud. Ingenieria</t>
-  </si>
-  <si>
     <t>Calculo III
 SALA 3pp</t>
   </si>
@@ -136,12 +126,17 @@
   <si>
     <t>Ayudantia 
 Calculo III</t>
+  </si>
+  <si>
+    <t>Logica
+Lab
+DC1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,12 +196,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -220,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -246,9 +235,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -310,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,26 +329,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,23 +364,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -587,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +612,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="5" t="s">
@@ -677,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="5" t="s">
@@ -697,11 +649,11 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>23</v>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
@@ -712,14 +664,14 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>23</v>
+      <c r="B8" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>21</v>
@@ -731,14 +683,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,14 +698,14 @@
         <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,7 +726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -786,7 +738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>